<commit_message>
LEctut : latest database files
</commit_message>
<xml_diff>
--- a/apps/lectut/scripts/old_db/exp.xlsx
+++ b/apps/lectut/scripts/old_db/exp.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="208" firstSheet="0" activeTab="0"/>
@@ -15,31 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="300">
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>faculty_id</t>
-  </si>
-  <si>
-    <t>course_id</t>
-  </si>
-  <si>
-    <t>file</t>
-  </si>
-  <si>
-    <t>topic</t>
-  </si>
-  <si>
-    <t>permission</t>
-  </si>
-  <si>
-    <t>timestamp</t>
-  </si>
-  <si>
-    <t>year</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="379">
   <si>
     <t>tashifph</t>
   </si>
@@ -623,36 +599,6 @@
     <t>2014-09-24 17:44:12</t>
   </si>
   <si>
-    <t>vivekfph</t>
-  </si>
-  <si>
-    <t>PH-005</t>
-  </si>
-  <si>
-    <t>PH-005 PH-005-MTE.pdf</t>
-  </si>
-  <si>
-    <t>2014-09-26 14:01:42</t>
-  </si>
-  <si>
-    <t>hem12fcy</t>
-  </si>
-  <si>
-    <t>CY-521</t>
-  </si>
-  <si>
-    <t>CY-521 msc_1styear_autumn_2013ETE.pdf</t>
-  </si>
-  <si>
-    <t>Thermodynamics and Surface Chemistry</t>
-  </si>
-  <si>
-    <t>2014-09-30 16:32:16</t>
-  </si>
-  <si>
-    <t>ETE  Autumn 201</t>
-  </si>
-  <si>
     <t>millifpt</t>
   </si>
   <si>
@@ -722,42 +668,6 @@
     <t>2014-11-19 12:03:22</t>
   </si>
   <si>
-    <t>CY-521 msc_1styear_autumn_2014ETE.pdf</t>
-  </si>
-  <si>
-    <t>Thermodynamics and surface chemistry</t>
-  </si>
-  <si>
-    <t>2014-11-20 11:57:48</t>
-  </si>
-  <si>
-    <t>Autumn  2014</t>
-  </si>
-  <si>
-    <t>CY-001</t>
-  </si>
-  <si>
-    <t>CY-001 CY001_ETE_Nov2014_kandpal.pdf</t>
-  </si>
-  <si>
-    <t>Quantum Mechanics Part Only</t>
-  </si>
-  <si>
-    <t>2014-11-21 11:15:35</t>
-  </si>
-  <si>
-    <t>Autumn-2014</t>
-  </si>
-  <si>
-    <t>CY-001 cy001_ete_autumn2014_question_paper.pdf</t>
-  </si>
-  <si>
-    <t>Physical Chemistry  question paper  Autumn 2014 </t>
-  </si>
-  <si>
-    <t>2014-11-21 11:27:45</t>
-  </si>
-  <si>
     <t>MI-103 marks MI-103 MECH.pdf</t>
   </si>
   <si>
@@ -773,148 +683,475 @@
     <t>anindfhs</t>
   </si>
   <si>
+    <t>IHS-04</t>
+  </si>
+  <si>
+    <t>IHS-04 IHS-04  notice for seeing answer scripts.docx</t>
+  </si>
+  <si>
+    <t>ENDSEM ANSWER SCRIPTS</t>
+  </si>
+  <si>
+    <t>2014-11-23 23:02:46</t>
+  </si>
+  <si>
+    <t>Autumn 2014</t>
+  </si>
+  <si>
+    <t>MI-103 New Microsoft Office Word Document.docx</t>
+  </si>
+  <si>
+    <t>End sem copy display</t>
+  </si>
+  <si>
+    <t>2014-11-24 10:12:21</t>
+  </si>
+  <si>
+    <t>umuksfce</t>
+  </si>
+  <si>
+    <t>CE-207</t>
+  </si>
+  <si>
+    <t>CE-207 FINAL_STATUS_CE207.xls</t>
+  </si>
+  <si>
+    <t>Total Final Marks</t>
+  </si>
+  <si>
+    <t>2014-11-25 21:57:41</t>
+  </si>
+  <si>
+    <t>2nd Year</t>
+  </si>
+  <si>
+    <t>HS-001A ETE OF HS 001 A.docx</t>
+  </si>
+  <si>
+    <t>ETE Answer Scripts</t>
+  </si>
+  <si>
+    <t>2014-11-27 08:14:06</t>
+  </si>
+  <si>
+    <t>IHS-04 IHS-04.xlsx</t>
+  </si>
+  <si>
+    <t>FINAL GRADES AUTUMN 2014</t>
+  </si>
+  <si>
+    <t>2014-11-30 12:26:20</t>
+  </si>
+  <si>
+    <t>balarfma</t>
+  </si>
+  <si>
+    <t>CS-102</t>
+  </si>
+  <si>
+    <t>CS-102 Surprise Quiz I.pdf</t>
+  </si>
+  <si>
+    <t>SQ 1</t>
+  </si>
+  <si>
+    <t>2015-02-15 01:08:02</t>
+  </si>
+  <si>
+    <t>2014-15</t>
+  </si>
+  <si>
+    <t>pmpradhan.fec</t>
+  </si>
+  <si>
+    <t>ECN-516</t>
+  </si>
+  <si>
+    <t>ECN-516 Class Test.pdf</t>
+  </si>
+  <si>
+    <t>Class Test dated Feb  9  2015</t>
+  </si>
+  <si>
+    <t>2015-02-17 14:45:11</t>
+  </si>
+  <si>
+    <t>sarkhel.fph</t>
+  </si>
+  <si>
+    <t>PHN-008</t>
+  </si>
+  <si>
+    <t>PHN-008 Display of MTE answer script_time-slot.pdf</t>
+  </si>
+  <si>
+    <t>Display of MTE Answer Scripts</t>
+  </si>
+  <si>
+    <t>2015-03-17 18:49:32</t>
+  </si>
+  <si>
+    <t>MI-362</t>
+  </si>
+  <si>
+    <t>MI-362 measurement PI marks.pdf</t>
+  </si>
+  <si>
+    <t>Practical marks  10 04 2015 </t>
+  </si>
+  <si>
+    <t>2015-04-10 18:27:47</t>
+  </si>
+  <si>
+    <t>ECN-516 MTE_2015_Exam_Paper.pdf</t>
+  </si>
+  <si>
+    <t>Mid-term Exam paper</t>
+  </si>
+  <si>
+    <t>2015-04-20 12:02:12</t>
+  </si>
+  <si>
+    <t>QUIZII-</t>
+  </si>
+  <si>
+    <t>QUIZII- Quiz II.pdf</t>
+  </si>
+  <si>
+    <t>2015-04-22 00:32:17</t>
+  </si>
+  <si>
+    <t>CS-102 Quiz III.pdf</t>
+  </si>
+  <si>
+    <t>Quiz 3</t>
+  </si>
+  <si>
+    <t>2015-04-22 23:30:33</t>
+  </si>
+  <si>
+    <t>subirfhs</t>
+  </si>
+  <si>
+    <t>HSN-01</t>
+  </si>
+  <si>
+    <t>HSN-01 HSN-01-Seating Plan ETE.pdf</t>
+  </si>
+  <si>
+    <t>Seating Plan ETE 1 May 2015</t>
+  </si>
+  <si>
+    <t>2015-04-30 12:20:46</t>
+  </si>
+  <si>
+    <t>duttafme</t>
+  </si>
+  <si>
+    <t>MI-106</t>
+  </si>
+  <si>
+    <t>MI-106 Notice.docx</t>
+  </si>
+  <si>
+    <t>ETE</t>
+  </si>
+  <si>
+    <t>2015-05-01 13:34:08</t>
+  </si>
+  <si>
+    <t>akmeqfeq</t>
+  </si>
+  <si>
+    <t>IEQ-01</t>
+  </si>
+  <si>
+    <t>IEQ-01 ieq01-marks-channeli.xlsx</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>2015-05-04 16:43:23</t>
+  </si>
+  <si>
+    <t>ssphf.fph</t>
+  </si>
+  <si>
+    <t>NT-604</t>
+  </si>
+  <si>
+    <t>NT-604 ETE Answers for NT-604.docx</t>
+  </si>
+  <si>
+    <t>Showing of ETE Answers</t>
+  </si>
+  <si>
+    <t>2015-05-05 23:15:45</t>
+  </si>
+  <si>
+    <t>swainfme</t>
+  </si>
+  <si>
+    <t>MI-108</t>
+  </si>
+  <si>
+    <t>MI-108 Showing End term answer script to student-(MI-108).pdf</t>
+  </si>
+  <si>
+    <t>Showing End term answer script to student- MI-108 </t>
+  </si>
+  <si>
+    <t>2015-05-06 06:56:51</t>
+  </si>
+  <si>
+    <t>aruphfph</t>
+  </si>
+  <si>
+    <t>PHN-006</t>
+  </si>
+  <si>
+    <t>PHN-006 PHN-006 Grades.pdf</t>
+  </si>
+  <si>
+    <t>Grades</t>
+  </si>
+  <si>
+    <t>2015-05-08 17:42:18</t>
+  </si>
+  <si>
     <t>HSS-02</t>
   </si>
   <si>
-    <t>HSS-02 HSS-02 notice for seeing answer scripts.docx</t>
-  </si>
-  <si>
-    <t>ENDSEM ANSWER SCRIPTS</t>
-  </si>
-  <si>
-    <t>2014-11-23 22:57:31</t>
-  </si>
-  <si>
-    <t>Autumn 2014</t>
-  </si>
-  <si>
-    <t>IHS-04</t>
-  </si>
-  <si>
-    <t>IHS-04 IHS-04  notice for seeing answer scripts.docx</t>
-  </si>
-  <si>
-    <t>2014-11-23 23:02:46</t>
-  </si>
-  <si>
-    <t>MI-103 New Microsoft Office Word Document.docx</t>
-  </si>
-  <si>
-    <t>End sem copy display</t>
-  </si>
-  <si>
-    <t>2014-11-24 10:12:21</t>
-  </si>
-  <si>
-    <t>PH-005 Notice_ETE_Answer_scripts.pdf</t>
-  </si>
-  <si>
-    <t>Answer  Scripts</t>
-  </si>
-  <si>
-    <t>2014-11-24 19:32:37</t>
-  </si>
-  <si>
-    <t>umuksfce</t>
-  </si>
-  <si>
-    <t>CE-207</t>
-  </si>
-  <si>
-    <t>CE-207 FINAL_STATUS_CE207.xls</t>
-  </si>
-  <si>
-    <t>Total Final Marks</t>
-  </si>
-  <si>
-    <t>2014-11-25 21:57:41</t>
-  </si>
-  <si>
-    <t>2nd Year</t>
-  </si>
-  <si>
-    <t>HS-001A ETE OF HS 001 A.docx</t>
-  </si>
-  <si>
-    <t>ETE Answer Scripts</t>
-  </si>
-  <si>
-    <t>2014-11-27 08:14:06</t>
-  </si>
-  <si>
-    <t>IHS-04 IHS-04.xlsx</t>
-  </si>
-  <si>
-    <t>FINAL GRADES AUTUMN 2014</t>
-  </si>
-  <si>
-    <t>2014-11-30 12:26:20</t>
-  </si>
-  <si>
-    <t>HSS-02 HSS-02 Sociology Autumn 2014.xlsx</t>
-  </si>
-  <si>
-    <t>2014-11-30 12:27:57</t>
-  </si>
-  <si>
-    <t>balarfma</t>
-  </si>
-  <si>
-    <t>CS-102</t>
-  </si>
-  <si>
-    <t>CS-102 Surprise Quiz I.pdf</t>
-  </si>
-  <si>
-    <t>SQ 1</t>
-  </si>
-  <si>
-    <t>2015-02-15 01:08:02</t>
-  </si>
-  <si>
-    <t>2014-15</t>
-  </si>
-  <si>
-    <t>pmpradhan.fec</t>
-  </si>
-  <si>
-    <t>ECN-516</t>
-  </si>
-  <si>
-    <t>ECN-516 Class Test.pdf</t>
-  </si>
-  <si>
-    <t>Class Test dated Feb  9  2015</t>
-  </si>
-  <si>
-    <t>2015-02-17 14:45:11</t>
-  </si>
-  <si>
-    <t>sarkhel.fph</t>
-  </si>
-  <si>
-    <t>PHN-008</t>
-  </si>
-  <si>
-    <t>PHN-008 Display of MTE answer script_time-slot.pdf</t>
-  </si>
-  <si>
-    <t>Display of MTE Answer Scripts</t>
-  </si>
-  <si>
-    <t>2015-03-17 18:49:32</t>
-  </si>
-  <si>
-    <t>MI-362</t>
-  </si>
-  <si>
-    <t>MI-362 measurement PI marks.pdf</t>
-  </si>
-  <si>
-    <t>Practical marks  10 04 2015 </t>
-  </si>
-  <si>
-    <t>2015-04-10 18:27:47</t>
+    <t>HSS-02 Grades HSS-02 Sociology Spring 2014-15.xlsx</t>
+  </si>
+  <si>
+    <t>Grades Spring 2015</t>
+  </si>
+  <si>
+    <t>2015-05-08 18:27:56</t>
+  </si>
+  <si>
+    <t>Spring 2015</t>
+  </si>
+  <si>
+    <t>IHS-09</t>
+  </si>
+  <si>
+    <t>IHS-09 Grades IHS-09 Science Technology &amp; Society Spring 2014-15.xlsx</t>
+  </si>
+  <si>
+    <t>2015-05-08 18:28:39</t>
+  </si>
+  <si>
+    <t>ECN-511</t>
+  </si>
+  <si>
+    <t>ECN-511 MTE_2014.pdf</t>
+  </si>
+  <si>
+    <t>Digital Communication Systems</t>
+  </si>
+  <si>
+    <t>2015-08-17 15:42:19</t>
+  </si>
+  <si>
+    <t>MI-407</t>
+  </si>
+  <si>
+    <t>MI-407 ct1 ans.pdf</t>
+  </si>
+  <si>
+    <t>class test 1</t>
+  </si>
+  <si>
+    <t>2015-08-24 20:58:51</t>
+  </si>
+  <si>
+    <t>CE-564 CE 564 M1&amp;2 Quiz 2015.PDF</t>
+  </si>
+  <si>
+    <t>M1 2 Quiz Solu</t>
+  </si>
+  <si>
+    <t>2015-09-03 12:51:53</t>
+  </si>
+  <si>
+    <t>prmdkfce</t>
+  </si>
+  <si>
+    <t>CEN-105</t>
+  </si>
+  <si>
+    <t>CEN-105 CE-102 MTE-II Q&amp;A Spring2011-12.pdf</t>
+  </si>
+  <si>
+    <t>MTE Q A</t>
+  </si>
+  <si>
+    <t>2015-09-11 11:22:30</t>
+  </si>
+  <si>
+    <t>2011-2012</t>
+  </si>
+  <si>
+    <t>bashefch</t>
+  </si>
+  <si>
+    <t>CEN-105 CE-102 MTE-II Q&amp;A.pdf</t>
+  </si>
+  <si>
+    <t>Sample test paper</t>
+  </si>
+  <si>
+    <t>2015-09-12 09:23:27</t>
+  </si>
+  <si>
+    <t>HSS-01</t>
+  </si>
+  <si>
+    <t>HSS-01 HSS 01 Economics - LHC 101.pdf</t>
+  </si>
+  <si>
+    <t>Seating Plan for MTE 24 Sept 2015 LHC 101</t>
+  </si>
+  <si>
+    <t>2015-09-15 11:17:28</t>
+  </si>
+  <si>
+    <t>HSS-01 HSS 01 Economics - LHC 102.pdf</t>
+  </si>
+  <si>
+    <t>Seating Plan for MTE 24 Sept 2015 LHC 102</t>
+  </si>
+  <si>
+    <t>2015-09-15 11:17:53</t>
+  </si>
+  <si>
+    <t>HSS-01 HSS 01 Economics - LHC 103.pdf</t>
+  </si>
+  <si>
+    <t>Seating Plan for MTE 24 Sept 2015 LHC 103</t>
+  </si>
+  <si>
+    <t>2015-09-15 11:18:14</t>
+  </si>
+  <si>
+    <t>HSS-01 HSS 01 Economics - LHC 104.pdf</t>
+  </si>
+  <si>
+    <t>Seating Plan for MTE 24 Sept 2015 LHC 104</t>
+  </si>
+  <si>
+    <t>2015-09-15 11:18:37</t>
+  </si>
+  <si>
+    <t>HSS-01 HSS 01 Economics - LHC 003.pdf</t>
+  </si>
+  <si>
+    <t>Seating Plan for MTE 24 Sept 2015 LHC 003</t>
+  </si>
+  <si>
+    <t>2015-09-15 11:19:55</t>
+  </si>
+  <si>
+    <t>HSS-01 HSS 01 Economics - LHC 004.pdf</t>
+  </si>
+  <si>
+    <t>Seating Plan for MTE 24 Sept 2015 LHC 004</t>
+  </si>
+  <si>
+    <t>2015-09-15 11:20:16</t>
+  </si>
+  <si>
+    <t>HSS-01 HSS 01 Economics - LHC 005.pdf</t>
+  </si>
+  <si>
+    <t>Seating Plan for MTE 24 Sept 2015 LHC 005</t>
+  </si>
+  <si>
+    <t>2015-09-15 11:20:35</t>
+  </si>
+  <si>
+    <t>HSS-01 HSS 01 Economics - LHC 006.pdf</t>
+  </si>
+  <si>
+    <t>Seating Plan for MTE 24 Sept 2015 LHC 006</t>
+  </si>
+  <si>
+    <t>2015-09-15 11:20:54</t>
+  </si>
+  <si>
+    <t>pjainfph</t>
+  </si>
+  <si>
+    <t>PHN-001</t>
+  </si>
+  <si>
+    <t>PHN-001 MTE-syllabus.pdf</t>
+  </si>
+  <si>
+    <t>Syllabus for MTE</t>
+  </si>
+  <si>
+    <t>2015-09-15 18:34:08</t>
+  </si>
+  <si>
+    <t>ram77fdm</t>
+  </si>
+  <si>
+    <t>IBM-309</t>
+  </si>
+  <si>
+    <t>IBM-309 Previous years question paper.pdf</t>
+  </si>
+  <si>
+    <t>Previous Years Question Papers </t>
+  </si>
+  <si>
+    <t>2015-09-15 22:36:38</t>
+  </si>
+  <si>
+    <t>rajacfce</t>
+  </si>
+  <si>
+    <t>mid tem exam</t>
+  </si>
+  <si>
+    <t>2015-09-15 23:28:31</t>
+  </si>
+  <si>
+    <t>CSN-103</t>
+  </si>
+  <si>
+    <t>CSN-103 samplecpp.pdf</t>
+  </si>
+  <si>
+    <t>Sample cpp paper</t>
+  </si>
+  <si>
+    <t>2015-09-16 12:39:10</t>
+  </si>
+  <si>
+    <t>2008-09</t>
+  </si>
+  <si>
+    <t>ECN-511 Quiz 1.pdf</t>
+  </si>
+  <si>
+    <t>Modules  1 - 3 </t>
+  </si>
+  <si>
+    <t>2015-09-18 19:27:39</t>
+  </si>
+  <si>
+    <t>CE-564 MTE2015_Paper&amp;Solutions.pdf</t>
+  </si>
+  <si>
+    <t>MTE 2015 paper</t>
+  </si>
+  <si>
+    <t>2015-09-23 14:28:38</t>
   </si>
 </sst>
 </file>
@@ -1015,10 +1252,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H69"/>
+  <dimension ref="A1:H90"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1026,214 +1263,214 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.47959183673469"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.515306122449"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.35204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="58.6785714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="42.4132653061225"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3214285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="61.1785714285714"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="43.3928571428571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="2.53571428571429"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.9642857142857"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.6326530612245"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
+      <c r="A1" s="0" t="n">
+        <v>2</v>
       </c>
       <c r="B1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="F2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="H2" s="0" t="s">
         <v>11</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="H3" s="0" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="0" t="s">
         <v>20</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="E5" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="F5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="H6" s="0" t="s">
         <v>30</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C7" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="F7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>38</v>
+      <c r="H7" s="0" t="n">
+        <v>2012</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="F8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="F8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="H8" s="0" t="n">
         <v>2012</v>
@@ -1241,97 +1478,97 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="F9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="F9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H9" s="0" t="n">
-        <v>2012</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B10" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="F10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="C11" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="F11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>57</v>
+      <c r="H11" s="0" t="n">
+        <v>2013</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H12" s="0" t="n">
         <v>2013</v>
@@ -1339,7 +1576,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>58</v>
@@ -1348,243 +1585,243 @@
         <v>59</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H13" s="0" t="n">
-        <v>2013</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B14" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="F14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="H14" s="0" t="s">
         <v>68</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="F14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B15" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="E15" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="F15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="F15" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="H15" s="0" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B16" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="F16" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F18" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B19" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="E19" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="F19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="H19" s="0" t="s">
         <v>91</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="F19" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="H19" s="0" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B20" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D20" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="E20" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="F20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="F20" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H20" s="0" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B21" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="E21" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="F21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="H21" s="0" t="s">
         <v>102</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="F21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B22" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C22" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="F22" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="H22" s="0" t="s">
-        <v>110</v>
+      <c r="H22" s="0" t="n">
+        <v>2013</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>58</v>
@@ -1593,16 +1830,16 @@
         <v>59</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="F23" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="H23" s="0" t="n">
         <v>2013</v>
@@ -1610,97 +1847,97 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>66</v>
+        <v>109</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>67</v>
+        <v>22</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F24" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="H24" s="0" t="n">
-        <v>2013</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F25" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B26" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="C26" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>121</v>
-      </c>
       <c r="E26" s="0" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="F26" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <v>2013</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="F27" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="H27" s="0" t="n">
         <v>2013</v>
@@ -1708,79 +1945,76 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B28" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="E28" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="C28" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>129</v>
-      </c>
       <c r="F28" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="H28" s="0" t="n">
-        <v>2013</v>
+        <v>125</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>30</v>
+        <v>127</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F29" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="F30" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>134</v>
@@ -1789,65 +2023,68 @@
         <v>135</v>
       </c>
       <c r="D31" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="H31" s="0" t="s">
         <v>139</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="F31" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B32" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C32" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="D32" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="E32" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="F32" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="H32" s="0" t="s">
-        <v>147</v>
+      <c r="H32" s="0" t="n">
+        <v>2013</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="F33" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="H33" s="0" t="n">
         <v>2013</v>
@@ -1855,195 +2092,195 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>40</v>
+        <v>127</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F34" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="H34" s="0" t="n">
-        <v>2013</v>
+        <v>148</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>134</v>
+        <v>149</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>135</v>
+        <v>150</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F35" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B36" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="C36" s="0" t="s">
+      <c r="H36" s="0" t="s">
         <v>158</v>
-      </c>
-      <c r="D36" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="E36" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="F36" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
+        <v>112</v>
+      </c>
+      <c r="B37" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="B37" s="0" t="s">
+      <c r="C37" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="F37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C37" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D37" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="E37" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="F37" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="H37" s="0" t="s">
-        <v>166</v>
+      <c r="H37" s="0" t="n">
+        <v>2014</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>117</v>
+        <v>154</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>167</v>
+        <v>1</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="F38" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="H38" s="0" t="n">
-        <v>2014</v>
+        <v>165</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>162</v>
+        <v>109</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>9</v>
+        <v>159</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="F39" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>117</v>
+        <v>169</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F40" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
+      </c>
+      <c r="H40" s="0" t="n">
+        <v>2014</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B41" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="E41" s="0" t="s">
         <v>177</v>
       </c>
-      <c r="C41" s="0" t="s">
+      <c r="F41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="D41" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="E41" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="F41" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>181</v>
       </c>
       <c r="H41" s="0" t="n">
         <v>2014</v>
@@ -2051,250 +2288,250 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B42" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="E42" s="0" t="s">
         <v>182</v>
       </c>
-      <c r="C42" s="0" t="s">
+      <c r="F42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="D42" s="0" t="s">
+      <c r="H42" s="0" t="s">
         <v>184</v>
-      </c>
-      <c r="E42" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="F42" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="H42" s="0" t="n">
-        <v>2014</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B43" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="E43" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="C43" s="0" t="s">
+      <c r="F43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="D43" s="0" t="s">
-        <v>189</v>
-      </c>
-      <c r="E43" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="F43" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="H43" s="0" t="s">
-        <v>192</v>
+      <c r="H43" s="0" t="n">
+        <v>2014</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>117</v>
+        <v>189</v>
       </c>
       <c r="C44" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="F44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="D44" s="0" t="s">
-        <v>194</v>
-      </c>
-      <c r="E44" s="0" t="s">
-        <v>195</v>
-      </c>
-      <c r="F44" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="H44" s="0" t="n">
-        <v>2014</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B45" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="E45" s="0" t="s">
         <v>197</v>
       </c>
-      <c r="C45" s="0" t="s">
+      <c r="F45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="D45" s="0" t="s">
+      <c r="H45" s="0" t="s">
         <v>199</v>
-      </c>
-      <c r="E45" s="0" t="s">
-        <v>200</v>
-      </c>
-      <c r="F45" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="B46" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="D46" s="0" t="s">
         <v>202</v>
       </c>
-      <c r="C46" s="0" t="s">
+      <c r="E46" s="0" t="s">
         <v>203</v>
       </c>
-      <c r="D46" s="0" t="s">
+      <c r="F46" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="E46" s="0" t="s">
-        <v>195</v>
-      </c>
-      <c r="F46" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>205</v>
+      <c r="H46" s="0" t="n">
+        <v>2014</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B47" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="C47" s="0" t="s">
         <v>206</v>
       </c>
-      <c r="C47" s="0" t="s">
+      <c r="D47" s="0" t="s">
         <v>207</v>
       </c>
-      <c r="D47" s="0" t="s">
+      <c r="E47" s="0" t="s">
         <v>208</v>
       </c>
-      <c r="E47" s="0" t="s">
+      <c r="F47" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G47" s="1" t="s">
         <v>209</v>
-      </c>
-      <c r="F47" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="H47" s="0" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="B48" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="F48" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G48" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="C48" s="0" t="s">
-        <v>213</v>
-      </c>
-      <c r="D48" s="0" t="s">
-        <v>214</v>
-      </c>
-      <c r="E48" s="0" t="s">
-        <v>215</v>
-      </c>
-      <c r="F48" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="H48" s="0" t="s">
-        <v>217</v>
+      <c r="H48" s="0" t="n">
+        <v>2014</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="F49" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="H49" s="0" t="n">
-        <v>2014</v>
+        <v>216</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>223</v>
+        <v>200</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>224</v>
+        <v>201</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>226</v>
+        <v>48</v>
       </c>
       <c r="F50" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>227</v>
+        <v>218</v>
+      </c>
+      <c r="H50" s="0" t="n">
+        <v>2014</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>117</v>
+        <v>200</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>229</v>
+        <v>48</v>
       </c>
       <c r="F51" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="H51" s="0" t="n">
         <v>2014</v>
@@ -2302,126 +2539,126 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="n">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="B52" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="D52" s="0" t="s">
         <v>223</v>
       </c>
-      <c r="C52" s="0" t="s">
-        <v>231</v>
-      </c>
-      <c r="D52" s="0" t="s">
-        <v>232</v>
-      </c>
       <c r="E52" s="0" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="F52" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>234</v>
+        <v>225</v>
+      </c>
+      <c r="H52" s="0" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="n">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="F53" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="H53" s="0" t="s">
-        <v>238</v>
+        <v>229</v>
+      </c>
+      <c r="H53" s="0" t="n">
+        <v>2014</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="n">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>206</v>
+        <v>230</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="F54" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="H54" s="0" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="n">
-        <v>142</v>
+        <v>155</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>239</v>
+        <v>213</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="F55" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="H55" s="0" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="n">
-        <v>143</v>
+        <v>156</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>56</v>
+        <v>240</v>
       </c>
       <c r="F56" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="H56" s="0" t="n">
         <v>2014</v>
@@ -2429,261 +2666,258 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>218</v>
+        <v>242</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>219</v>
+        <v>243</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>56</v>
+        <v>245</v>
       </c>
       <c r="F57" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="H57" s="0" t="n">
-        <v>2014</v>
+        <v>246</v>
+      </c>
+      <c r="H57" s="0" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
-        <v>145</v>
+        <v>159</v>
       </c>
       <c r="B58" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>249</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>250</v>
+      </c>
+      <c r="E58" s="0" t="s">
         <v>251</v>
       </c>
-      <c r="C58" s="0" t="s">
+      <c r="F58" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G58" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="D58" s="0" t="s">
-        <v>253</v>
-      </c>
-      <c r="E58" s="0" t="s">
-        <v>254</v>
-      </c>
-      <c r="F58" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="H58" s="0" t="s">
-        <v>256</v>
+      <c r="H58" s="0" t="n">
+        <v>2015</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="n">
-        <v>146</v>
+        <v>162</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C59" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="E59" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="F59" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G59" s="1" t="s">
         <v>257</v>
-      </c>
-      <c r="D59" s="0" t="s">
-        <v>258</v>
-      </c>
-      <c r="E59" s="0" t="s">
-        <v>254</v>
-      </c>
-      <c r="F59" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="H59" s="0" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
-        <v>147</v>
+        <v>163</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>219</v>
+        <v>258</v>
       </c>
       <c r="D60" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="E60" s="0" t="s">
         <v>260</v>
       </c>
-      <c r="E60" s="0" t="s">
+      <c r="F60" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G60" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="F60" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>262</v>
-      </c>
       <c r="H60" s="0" t="n">
-        <v>2014</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
-        <v>149</v>
+        <v>164</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>202</v>
+        <v>248</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>203</v>
+        <v>249</v>
       </c>
       <c r="D61" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="E61" s="0" t="s">
         <v>263</v>
       </c>
-      <c r="E61" s="0" t="s">
+      <c r="F61" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G61" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="F61" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>265</v>
+      <c r="H61" s="0" t="n">
+        <v>2015</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="B62" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="D62" s="0" t="s">
         <v>266</v>
       </c>
-      <c r="C62" s="0" t="s">
+      <c r="E62" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F62" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G62" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="D62" s="0" t="s">
-        <v>268</v>
-      </c>
-      <c r="E62" s="0" t="s">
-        <v>269</v>
-      </c>
-      <c r="F62" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>270</v>
-      </c>
       <c r="H62" s="0" t="s">
-        <v>271</v>
+        <v>247</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="n">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>223</v>
+        <v>242</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>231</v>
+        <v>243</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="F63" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>274</v>
+        <v>270</v>
+      </c>
+      <c r="H63" s="0" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="n">
-        <v>156</v>
+        <v>170</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>251</v>
+        <v>271</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>257</v>
+        <v>272</v>
       </c>
       <c r="D64" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="E64" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="F64" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G64" s="1" t="s">
         <v>275</v>
-      </c>
-      <c r="E64" s="0" t="s">
-        <v>276</v>
-      </c>
-      <c r="F64" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="H64" s="0" t="n">
-        <v>2014</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="n">
-        <v>157</v>
+        <v>172</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>251</v>
+        <v>276</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>252</v>
+        <v>277</v>
       </c>
       <c r="D65" s="0" t="s">
         <v>278</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="F65" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="H65" s="0" t="n">
-        <v>2014</v>
+        <v>280</v>
+      </c>
+      <c r="H65" s="0" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="n">
-        <v>158</v>
+        <v>173</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="F66" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="H66" s="0" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="n">
-        <v>159</v>
+        <v>177</v>
       </c>
       <c r="B67" s="0" t="s">
         <v>286</v>
@@ -2709,7 +2943,7 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="n">
-        <v>162</v>
+        <v>178</v>
       </c>
       <c r="B68" s="0" t="s">
         <v>291</v>
@@ -2732,27 +2966,537 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="n">
-        <v>163</v>
+        <v>180</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>218</v>
+        <v>296</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="F69" s="0" t="n">
         <v>0</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="H69" s="0" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="n">
+        <v>181</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="D70" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="E70" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="F70" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="H70" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="n">
+        <v>182</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="C71" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="D71" s="0" t="s">
+        <v>307</v>
+      </c>
+      <c r="E71" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="F71" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="H71" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="n">
+        <v>183</v>
+      </c>
+      <c r="B72" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="D72" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="E72" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="F72" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="H72" s="0" t="n">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="n">
+        <v>184</v>
+      </c>
+      <c r="B73" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="C73" s="0" t="s">
+        <v>313</v>
+      </c>
+      <c r="D73" s="0" t="s">
+        <v>314</v>
+      </c>
+      <c r="E73" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="F73" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="H73" s="0" t="n">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="n">
+        <v>186</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="C74" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="D74" s="0" t="s">
+        <v>317</v>
+      </c>
+      <c r="E74" s="0" t="s">
+        <v>318</v>
+      </c>
+      <c r="F74" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="H74" s="0" t="n">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="n">
+        <v>187</v>
+      </c>
+      <c r="B75" s="0" t="s">
+        <v>320</v>
+      </c>
+      <c r="C75" s="0" t="s">
+        <v>321</v>
+      </c>
+      <c r="D75" s="0" t="s">
+        <v>322</v>
+      </c>
+      <c r="E75" s="0" t="s">
+        <v>323</v>
+      </c>
+      <c r="F75" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="H75" s="0" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="n">
+        <v>188</v>
+      </c>
+      <c r="B76" s="0" t="s">
+        <v>326</v>
+      </c>
+      <c r="C76" s="0" t="s">
+        <v>321</v>
+      </c>
+      <c r="D76" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="E76" s="0" t="s">
+        <v>328</v>
+      </c>
+      <c r="F76" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="n">
+        <v>193</v>
+      </c>
+      <c r="B77" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="C77" s="0" t="s">
+        <v>330</v>
+      </c>
+      <c r="D77" s="0" t="s">
+        <v>331</v>
+      </c>
+      <c r="E77" s="0" t="s">
+        <v>332</v>
+      </c>
+      <c r="F77" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="n">
+        <v>194</v>
+      </c>
+      <c r="B78" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="C78" s="0" t="s">
+        <v>330</v>
+      </c>
+      <c r="D78" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="E78" s="0" t="s">
+        <v>335</v>
+      </c>
+      <c r="F78" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="n">
+        <v>195</v>
+      </c>
+      <c r="B79" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="C79" s="0" t="s">
+        <v>330</v>
+      </c>
+      <c r="D79" s="0" t="s">
+        <v>337</v>
+      </c>
+      <c r="E79" s="0" t="s">
+        <v>338</v>
+      </c>
+      <c r="F79" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="n">
+        <v>196</v>
+      </c>
+      <c r="B80" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="C80" s="0" t="s">
+        <v>330</v>
+      </c>
+      <c r="D80" s="0" t="s">
+        <v>340</v>
+      </c>
+      <c r="E80" s="0" t="s">
+        <v>341</v>
+      </c>
+      <c r="F80" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="n">
+        <v>197</v>
+      </c>
+      <c r="B81" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="C81" s="0" t="s">
+        <v>330</v>
+      </c>
+      <c r="D81" s="0" t="s">
+        <v>343</v>
+      </c>
+      <c r="E81" s="0" t="s">
+        <v>344</v>
+      </c>
+      <c r="F81" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="n">
+        <v>198</v>
+      </c>
+      <c r="B82" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="C82" s="0" t="s">
+        <v>330</v>
+      </c>
+      <c r="D82" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="E82" s="0" t="s">
+        <v>347</v>
+      </c>
+      <c r="F82" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="n">
+        <v>199</v>
+      </c>
+      <c r="B83" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="C83" s="0" t="s">
+        <v>330</v>
+      </c>
+      <c r="D83" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="E83" s="0" t="s">
+        <v>350</v>
+      </c>
+      <c r="F83" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="B84" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="C84" s="0" t="s">
+        <v>330</v>
+      </c>
+      <c r="D84" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="E84" s="0" t="s">
+        <v>353</v>
+      </c>
+      <c r="F84" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="n">
+        <v>201</v>
+      </c>
+      <c r="B85" s="0" t="s">
+        <v>355</v>
+      </c>
+      <c r="C85" s="0" t="s">
+        <v>356</v>
+      </c>
+      <c r="D85" s="0" t="s">
+        <v>357</v>
+      </c>
+      <c r="E85" s="0" t="s">
+        <v>358</v>
+      </c>
+      <c r="F85" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="n">
+        <v>202</v>
+      </c>
+      <c r="B86" s="0" t="s">
+        <v>360</v>
+      </c>
+      <c r="C86" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="D86" s="0" t="s">
+        <v>362</v>
+      </c>
+      <c r="E86" s="0" t="s">
+        <v>363</v>
+      </c>
+      <c r="F86" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="n">
+        <v>203</v>
+      </c>
+      <c r="B87" s="0" t="s">
+        <v>365</v>
+      </c>
+      <c r="C87" s="0" t="s">
+        <v>321</v>
+      </c>
+      <c r="D87" s="0" t="s">
+        <v>322</v>
+      </c>
+      <c r="E87" s="0" t="s">
+        <v>366</v>
+      </c>
+      <c r="F87" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="H87" s="0" t="n">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="n">
+        <v>204</v>
+      </c>
+      <c r="B88" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="C88" s="0" t="s">
+        <v>368</v>
+      </c>
+      <c r="D88" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="E88" s="0" t="s">
+        <v>370</v>
+      </c>
+      <c r="F88" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="H88" s="0" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="n">
+        <v>205</v>
+      </c>
+      <c r="B89" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="C89" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="D89" s="0" t="s">
+        <v>373</v>
+      </c>
+      <c r="E89" s="0" t="s">
+        <v>374</v>
+      </c>
+      <c r="F89" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="H89" s="0" t="n">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="n">
+        <v>206</v>
+      </c>
+      <c r="B90" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="C90" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="D90" s="0" t="s">
+        <v>376</v>
+      </c>
+      <c r="E90" s="0" t="s">
+        <v>377</v>
+      </c>
+      <c r="F90" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="H90" s="0" t="n">
         <v>2015</v>
       </c>
     </row>

</xml_diff>